<commit_message>
Changing the script logic
</commit_message>
<xml_diff>
--- a/Утиль.xlsx
+++ b/Утиль.xlsx
@@ -391,10 +391,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C29"/>
+      <selection activeCell="C34" sqref="C2:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -434,7 +434,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Залит, GPRS</t>
+          <t>Механические повреждения, Принтер</t>
         </is>
       </c>
     </row>
@@ -468,7 +468,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Залит, CTLS</t>
+          <t>Залит, Принтер</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Неустранимые загрязнения, CTLS</t>
+          <t>Следы жизнедеятельности, GPRS</t>
         </is>
       </c>
     </row>
@@ -502,7 +502,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Следы жизнедеятельности, Tamper</t>
+          <t>Неустранимые загрязнения, Принтер</t>
         </is>
       </c>
     </row>
@@ -519,7 +519,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Залит, GPRS</t>
+          <t>Следы жизнедеятельности, GPRS</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Залит, CTLS</t>
+          <t>Залит, Tamper</t>
         </is>
       </c>
     </row>
@@ -553,7 +553,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Механические повреждения, Дефект клавиатуры</t>
+          <t>Залит, Дефект клавиатуры</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Залит, Принтер</t>
+          <t>Неустранимые загрязнения, Дефект клавиатуры</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Залит, Tamper</t>
+          <t>Механические повреждения, Принтер</t>
         </is>
       </c>
     </row>
@@ -604,7 +604,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Следы жизнедеятельности, Дефект экрана</t>
+          <t>Механические повреждения, CTLS</t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Неустранимые загрязнения, CTLS</t>
+          <t>Залит, Принтер</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Следы жизнедеятельности, Порт питания</t>
+          <t>Неустранимые загрязнения, Дефект клавиатуры</t>
         </is>
       </c>
     </row>
@@ -672,7 +672,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Неустранимые загрязнения, GPRS</t>
+          <t>Залит, Принтер</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Неустранимые загрязнения, Дефект экрана</t>
+          <t>Залит, Порт питания</t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Залит, CTLS</t>
+          <t>Механические повреждения, Tamper</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Залит, GPRS</t>
+          <t>Механические повреждения, GPRS</t>
         </is>
       </c>
     </row>
@@ -740,7 +740,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Неустранимые загрязнения, Дефект клавиатуры</t>
+          <t>Механические повреждения, Дефект экрана</t>
         </is>
       </c>
     </row>
@@ -757,7 +757,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Залит, Tamper</t>
+          <t>Неустранимые загрязнения, Принтер</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Неустранимые загрязнения, Принтер</t>
+          <t>Залит, CTLS</t>
         </is>
       </c>
     </row>
@@ -808,7 +808,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Неустранимые загрязнения, Дефект клавиатуры</t>
+          <t>Залит, Alert</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Следы жизнедеятельности, CTLS</t>
+          <t>Механические повреждения, CTLS</t>
         </is>
       </c>
     </row>
@@ -842,7 +842,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Механические повреждения, Tamper</t>
+          <t>Залит, CTLS</t>
         </is>
       </c>
     </row>
@@ -859,7 +859,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Механические повреждения, Дефект экрана</t>
+          <t>Неустранимые загрязнения, Дефект клавиатуры</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Следы жизнедеятельности, Принтер</t>
+          <t>Залит, GPRS</t>
         </is>
       </c>
     </row>
@@ -893,7 +893,24 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Следы жизнедеятельности, CTLS</t>
+          <t>Механические повреждения, CTLS</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Castles</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>12345345687u</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Неустранимые загрязнения</t>
         </is>
       </c>
     </row>

</xml_diff>